<commit_message>
add setDev1Percentage and delete redundant
</commit_message>
<xml_diff>
--- a/Notify_ErrorCode.xlsx
+++ b/Notify_ErrorCode.xlsx
@@ -141,27 +141,27 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>[endDisk:String, diskId:Integer, diskRes:Integer, winnerPayAmountList:List2]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>List2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a list of List</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>List1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[saveGameResultByOracleRes:String, jsonIndex:Integer, gameDiskIdList:List1, gameDiskResultList:List]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Note</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[saveGameResultByOracleRes:String, jsonIndex:Integer, gameDiskIdList:List1, gameDiskResultList:List]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[endDisk:String, diskId:Integer, diskRes:Integer, winnerPayAmountList:List2]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>List2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>List</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>a list of List</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -233,15 +233,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -526,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:XFD26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -538,11 +538,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -677,46 +677,46 @@
       </c>
     </row>
     <row r="14" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-    </row>
-    <row r="15" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+    </row>
+    <row r="15" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+    <row r="17" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+    <row r="18" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
+    <row r="19" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
+    <row r="20" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
+    <row r="21" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -731,7 +731,7 @@
     </row>
     <row r="25" spans="1:3" s="6" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -740,41 +740,52 @@
       </c>
     </row>
     <row r="27" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
+      <c r="A27" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
     </row>
     <row r="28" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C28" s="9"/>
+      <c r="C28" s="7"/>
     </row>
     <row r="29" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C29" s="9"/>
+        <v>33</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="7"/>
     </row>
     <row r="30" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B30" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="9"/>
+      <c r="C30" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A24:XFD24"/>
+    <mergeCell ref="A26:XFD26"/>
+    <mergeCell ref="A25:XFD25"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A16:XFD16"/>
+    <mergeCell ref="A17:XFD17"/>
+    <mergeCell ref="A18:XFD18"/>
     <mergeCell ref="A23:XFD23"/>
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="A19:XFD19"/>
@@ -782,17 +793,6 @@
     <mergeCell ref="A20:XFD20"/>
     <mergeCell ref="A21:XFD21"/>
     <mergeCell ref="A22:XFD22"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A16:XFD16"/>
-    <mergeCell ref="A17:XFD17"/>
-    <mergeCell ref="A18:XFD18"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A24:XFD24"/>
-    <mergeCell ref="A26:XFD26"/>
-    <mergeCell ref="A25:XFD25"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add migrateContract method and add it in readme and mofity the Notify_ErrorCode.xlsx
</commit_message>
<xml_diff>
--- a/Notify_ErrorCode.xlsx
+++ b/Notify_ErrorCode.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
   <si>
     <t>Error</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -162,6 +162,18 @@
   </si>
   <si>
     <t>Note</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[Migrate Contract successfully:String, Dev1:Address]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Error</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>migrateContract: MigrateContractError, transfer ONG to new contract error</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -217,7 +229,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -234,14 +246,17 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -524,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:XFD22"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -677,122 +692,141 @@
       </c>
     </row>
     <row r="14" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="1">
+        <v>501</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-    </row>
-    <row r="15" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+    </row>
+    <row r="16" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
+    <row r="20" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
+    <row r="21" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
+    <row r="22" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+    <row r="23" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+    <row r="24" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+    <row r="25" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="6" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+    <row r="26" spans="1:3" s="9" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+    <row r="27" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
+    <row r="28" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+    </row>
+    <row r="29" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="11"/>
-      <c r="C27" s="11"/>
-    </row>
-    <row r="28" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C28" s="7"/>
-    </row>
-    <row r="29" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C29" s="7"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
     </row>
     <row r="30" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="7"/>
+    </row>
+    <row r="31" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="7"/>
+    </row>
+    <row r="32" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="B32" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="7"/>
+      <c r="C32" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="A27:C27"/>
+  <mergeCells count="19">
     <mergeCell ref="A24:XFD24"/>
-    <mergeCell ref="A26:XFD26"/>
-    <mergeCell ref="A25:XFD25"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="A20:XFD20"/>
+    <mergeCell ref="A16:XFD16"/>
+    <mergeCell ref="A21:XFD21"/>
+    <mergeCell ref="A22:XFD22"/>
+    <mergeCell ref="A23:XFD23"/>
+    <mergeCell ref="A28:C28"/>
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A16:XFD16"/>
+    <mergeCell ref="A15:C15"/>
     <mergeCell ref="A17:XFD17"/>
     <mergeCell ref="A18:XFD18"/>
-    <mergeCell ref="A23:XFD23"/>
-    <mergeCell ref="B29:C29"/>
     <mergeCell ref="A19:XFD19"/>
-    <mergeCell ref="A15:XFD15"/>
-    <mergeCell ref="A20:XFD20"/>
-    <mergeCell ref="A21:XFD21"/>
-    <mergeCell ref="A22:XFD22"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="A25:XFD25"/>
+    <mergeCell ref="A27:XFD27"/>
+    <mergeCell ref="A26:XFD26"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>